<commit_message>
added REL on apease
</commit_message>
<xml_diff>
--- a/BCW/BCIO_BCW_Defs.xlsx
+++ b/BCW/BCIO_BCW_Defs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rober\Documents\GitHub\ontologies\BCW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DE32E3F-A48C-4099-9991-E93314D67C90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12426F60-0523-4424-81B5-062B77A2FB66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="681" uniqueCount="363">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="673" uniqueCount="359">
   <si>
     <t>ID</t>
   </si>
@@ -697,24 +697,9 @@
     <t>This includes use of any kind of reward, including financial, social and material. It also includes prevention or cessationl of naturally occuring negative experiences.</t>
   </si>
   <si>
-    <t>BCIO:040000</t>
-  </si>
-  <si>
-    <t>individual human activity</t>
-  </si>
-  <si>
-    <t>A process that is produced by a person.</t>
-  </si>
-  <si>
-    <t>Something that someone does, whether it be mental or physical.</t>
-  </si>
-  <si>
     <t>Upper level</t>
   </si>
   <si>
-    <t>Obsolete</t>
-  </si>
-  <si>
     <t>BCIO:036000</t>
   </si>
   <si>
@@ -1109,6 +1094,9 @@
   </si>
   <si>
     <t>REL 'can influence'</t>
+  </si>
+  <si>
+    <t>REL 'can be a standard for evaluation of'</t>
   </si>
 </sst>
 </file>
@@ -1129,7 +1117,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1139,11 +1127,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF2F4F4F"/>
       </patternFill>
     </fill>
   </fills>
@@ -1159,11 +1142,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1466,7 +1448,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AC60"/>
+  <dimension ref="A1:AD59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="M2" sqref="M2"/>
@@ -1474,7 +1456,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1506,64 +1488,67 @@
         <v>9</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>362</v>
+        <v>357</v>
       </c>
       <c r="M1" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>27</v>
       </c>
@@ -1595,28 +1580,29 @@
       <c r="O2" s="2"/>
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
-      <c r="R2" s="2" t="s">
+      <c r="R2" s="2"/>
+      <c r="S2" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="S2" s="2"/>
       <c r="T2" s="2"/>
-      <c r="U2" s="2" t="s">
+      <c r="U2" s="2"/>
+      <c r="V2" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="V2" s="2"/>
-      <c r="W2" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="X2" s="2"/>
+      <c r="W2" s="2"/>
+      <c r="X2" s="2" t="s">
+        <v>36</v>
+      </c>
       <c r="Y2" s="2"/>
-      <c r="Z2" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="AA2" s="2"/>
+      <c r="Z2" s="2"/>
+      <c r="AA2" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="AB2" s="2"/>
       <c r="AC2" s="2"/>
-    </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD2" s="2"/>
+    </row>
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>38</v>
       </c>
@@ -1648,32 +1634,33 @@
       <c r="O3" s="2"/>
       <c r="P3" s="2"/>
       <c r="Q3" s="2"/>
-      <c r="R3" s="2" t="s">
+      <c r="R3" s="2"/>
+      <c r="S3" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="S3" s="2" t="s">
+      <c r="T3" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="T3" s="2"/>
-      <c r="U3" s="2" t="s">
+      <c r="U3" s="2"/>
+      <c r="V3" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="V3" s="2"/>
-      <c r="W3" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="X3" s="2"/>
-      <c r="Y3" s="2" t="s">
+      <c r="W3" s="2"/>
+      <c r="X3" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y3" s="2"/>
+      <c r="Z3" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="Z3" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="AA3" s="2"/>
+      <c r="AA3" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="AB3" s="2"/>
       <c r="AC3" s="2"/>
-    </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD3" s="2"/>
+    </row>
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>45</v>
       </c>
@@ -1705,30 +1692,31 @@
       <c r="O4" s="2"/>
       <c r="P4" s="2"/>
       <c r="Q4" s="2"/>
-      <c r="R4" s="2" t="s">
+      <c r="R4" s="2"/>
+      <c r="S4" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="S4" s="2" t="s">
+      <c r="T4" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="T4" s="2"/>
-      <c r="U4" s="2" t="s">
+      <c r="U4" s="2"/>
+      <c r="V4" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="V4" s="2"/>
-      <c r="W4" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="X4" s="2"/>
+      <c r="W4" s="2"/>
+      <c r="X4" s="2" t="s">
+        <v>36</v>
+      </c>
       <c r="Y4" s="2"/>
-      <c r="Z4" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="AA4" s="2"/>
+      <c r="Z4" s="2"/>
+      <c r="AA4" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="AB4" s="2"/>
       <c r="AC4" s="2"/>
-    </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD4" s="2"/>
+    </row>
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>51</v>
       </c>
@@ -1760,28 +1748,29 @@
       <c r="O5" s="2"/>
       <c r="P5" s="2"/>
       <c r="Q5" s="2"/>
-      <c r="R5" s="2" t="s">
+      <c r="R5" s="2"/>
+      <c r="S5" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="S5" s="2"/>
       <c r="T5" s="2"/>
-      <c r="U5" s="2" t="s">
+      <c r="U5" s="2"/>
+      <c r="V5" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="V5" s="2"/>
-      <c r="W5" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="X5" s="2"/>
+      <c r="W5" s="2"/>
+      <c r="X5" s="2" t="s">
+        <v>36</v>
+      </c>
       <c r="Y5" s="2"/>
-      <c r="Z5" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="AA5" s="2"/>
+      <c r="Z5" s="2"/>
+      <c r="AA5" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="AB5" s="2"/>
       <c r="AC5" s="2"/>
-    </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD5" s="2"/>
+    </row>
+    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>60</v>
       </c>
@@ -1813,30 +1802,31 @@
       <c r="O6" s="2"/>
       <c r="P6" s="2"/>
       <c r="Q6" s="2"/>
-      <c r="R6" s="2" t="s">
+      <c r="R6" s="2"/>
+      <c r="S6" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="S6" s="2" t="s">
+      <c r="T6" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="T6" s="2"/>
-      <c r="U6" s="2" t="s">
+      <c r="U6" s="2"/>
+      <c r="V6" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="V6" s="2"/>
-      <c r="W6" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="X6" s="2"/>
+      <c r="W6" s="2"/>
+      <c r="X6" s="2" t="s">
+        <v>36</v>
+      </c>
       <c r="Y6" s="2"/>
-      <c r="Z6" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="AA6" s="2"/>
+      <c r="Z6" s="2"/>
+      <c r="AA6" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="AB6" s="2"/>
       <c r="AC6" s="2"/>
-    </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD6" s="2"/>
+    </row>
+    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>67</v>
       </c>
@@ -1868,30 +1858,31 @@
       <c r="O7" s="2"/>
       <c r="P7" s="2"/>
       <c r="Q7" s="2"/>
-      <c r="R7" s="2" t="s">
+      <c r="R7" s="2"/>
+      <c r="S7" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="S7" s="2" t="s">
+      <c r="T7" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="T7" s="2"/>
-      <c r="U7" s="2" t="s">
+      <c r="U7" s="2"/>
+      <c r="V7" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="V7" s="2"/>
-      <c r="W7" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="X7" s="2"/>
+      <c r="W7" s="2"/>
+      <c r="X7" s="2" t="s">
+        <v>36</v>
+      </c>
       <c r="Y7" s="2"/>
-      <c r="Z7" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="AA7" s="2"/>
+      <c r="Z7" s="2"/>
+      <c r="AA7" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="AB7" s="2"/>
       <c r="AC7" s="2"/>
-    </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD7" s="2"/>
+    </row>
+    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>73</v>
       </c>
@@ -1923,30 +1914,31 @@
       <c r="O8" s="2"/>
       <c r="P8" s="2"/>
       <c r="Q8" s="2"/>
-      <c r="R8" s="2" t="s">
+      <c r="R8" s="2"/>
+      <c r="S8" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="S8" s="2" t="s">
+      <c r="T8" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="T8" s="2"/>
-      <c r="U8" s="2" t="s">
+      <c r="U8" s="2"/>
+      <c r="V8" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="V8" s="2"/>
-      <c r="W8" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="X8" s="2"/>
+      <c r="W8" s="2"/>
+      <c r="X8" s="2" t="s">
+        <v>36</v>
+      </c>
       <c r="Y8" s="2"/>
-      <c r="Z8" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="AA8" s="2"/>
+      <c r="Z8" s="2"/>
+      <c r="AA8" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="AB8" s="2"/>
       <c r="AC8" s="2"/>
-    </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD8" s="2"/>
+    </row>
+    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>79</v>
       </c>
@@ -1978,30 +1970,31 @@
       <c r="O9" s="2"/>
       <c r="P9" s="2"/>
       <c r="Q9" s="2"/>
-      <c r="R9" s="2" t="s">
+      <c r="R9" s="2"/>
+      <c r="S9" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="S9" s="2" t="s">
+      <c r="T9" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="T9" s="2"/>
-      <c r="U9" s="2" t="s">
+      <c r="U9" s="2"/>
+      <c r="V9" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="V9" s="2"/>
-      <c r="W9" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="X9" s="2"/>
+      <c r="W9" s="2"/>
+      <c r="X9" s="2" t="s">
+        <v>36</v>
+      </c>
       <c r="Y9" s="2"/>
-      <c r="Z9" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="AA9" s="2"/>
+      <c r="Z9" s="2"/>
+      <c r="AA9" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="AB9" s="2"/>
       <c r="AC9" s="2"/>
-    </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD9" s="2"/>
+    </row>
+    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>85</v>
       </c>
@@ -2034,25 +2027,26 @@
       <c r="P10" s="2"/>
       <c r="Q10" s="2"/>
       <c r="R10" s="2"/>
-      <c r="S10" s="2" t="s">
+      <c r="S10" s="2"/>
+      <c r="T10" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="T10" s="2"/>
       <c r="U10" s="2"/>
       <c r="V10" s="2"/>
-      <c r="W10" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="X10" s="2"/>
+      <c r="W10" s="2"/>
+      <c r="X10" s="2" t="s">
+        <v>36</v>
+      </c>
       <c r="Y10" s="2"/>
-      <c r="Z10" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="AA10" s="2"/>
+      <c r="Z10" s="2"/>
+      <c r="AA10" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="AB10" s="2"/>
       <c r="AC10" s="2"/>
-    </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD10" s="2"/>
+    </row>
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>91</v>
       </c>
@@ -2085,29 +2079,30 @@
       <c r="P11" s="2"/>
       <c r="Q11" s="2"/>
       <c r="R11" s="2"/>
-      <c r="S11" s="2" t="s">
+      <c r="S11" s="2"/>
+      <c r="T11" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="T11" s="2"/>
-      <c r="U11" s="2" t="s">
+      <c r="U11" s="2"/>
+      <c r="V11" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="V11" s="2"/>
-      <c r="W11" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="X11" s="2"/>
-      <c r="Y11" s="2" t="s">
+      <c r="W11" s="2"/>
+      <c r="X11" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y11" s="2"/>
+      <c r="Z11" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="Z11" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="AA11" s="2"/>
+      <c r="AA11" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="AB11" s="2"/>
       <c r="AC11" s="2"/>
-    </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD11" s="2"/>
+    </row>
+    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>97</v>
       </c>
@@ -2139,28 +2134,29 @@
       <c r="O12" s="2"/>
       <c r="P12" s="2"/>
       <c r="Q12" s="2"/>
-      <c r="R12" s="2" t="s">
+      <c r="R12" s="2"/>
+      <c r="S12" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="S12" s="2" t="s">
+      <c r="T12" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="T12" s="2"/>
       <c r="U12" s="2"/>
       <c r="V12" s="2"/>
-      <c r="W12" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="X12" s="2"/>
+      <c r="W12" s="2"/>
+      <c r="X12" s="2" t="s">
+        <v>36</v>
+      </c>
       <c r="Y12" s="2"/>
-      <c r="Z12" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="AA12" s="2"/>
+      <c r="Z12" s="2"/>
+      <c r="AA12" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="AB12" s="2"/>
       <c r="AC12" s="2"/>
-    </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD12" s="2"/>
+    </row>
+    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>102</v>
       </c>
@@ -2192,30 +2188,31 @@
       <c r="O13" s="2"/>
       <c r="P13" s="2"/>
       <c r="Q13" s="2"/>
-      <c r="R13" s="2" t="s">
+      <c r="R13" s="2"/>
+      <c r="S13" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="S13" s="2" t="s">
+      <c r="T13" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="T13" s="2"/>
-      <c r="U13" s="2" t="s">
+      <c r="U13" s="2"/>
+      <c r="V13" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="V13" s="2"/>
-      <c r="W13" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="X13" s="2"/>
+      <c r="W13" s="2"/>
+      <c r="X13" s="2" t="s">
+        <v>36</v>
+      </c>
       <c r="Y13" s="2"/>
-      <c r="Z13" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="AA13" s="2"/>
+      <c r="Z13" s="2"/>
+      <c r="AA13" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="AB13" s="2"/>
       <c r="AC13" s="2"/>
-    </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD13" s="2"/>
+    </row>
+    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>108</v>
       </c>
@@ -2247,28 +2244,29 @@
       <c r="O14" s="2"/>
       <c r="P14" s="2"/>
       <c r="Q14" s="2"/>
-      <c r="R14" s="2" t="s">
+      <c r="R14" s="2"/>
+      <c r="S14" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="S14" s="2" t="s">
+      <c r="T14" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="T14" s="2"/>
       <c r="U14" s="2"/>
       <c r="V14" s="2"/>
-      <c r="W14" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="X14" s="2"/>
+      <c r="W14" s="2"/>
+      <c r="X14" s="2" t="s">
+        <v>36</v>
+      </c>
       <c r="Y14" s="2"/>
-      <c r="Z14" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="AA14" s="2"/>
+      <c r="Z14" s="2"/>
+      <c r="AA14" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="AB14" s="2"/>
       <c r="AC14" s="2"/>
-    </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD14" s="2"/>
+    </row>
+    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>113</v>
       </c>
@@ -2300,28 +2298,29 @@
       <c r="O15" s="2"/>
       <c r="P15" s="2"/>
       <c r="Q15" s="2"/>
-      <c r="R15" s="2" t="s">
+      <c r="R15" s="2"/>
+      <c r="S15" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="S15" s="2" t="s">
+      <c r="T15" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="T15" s="2"/>
       <c r="U15" s="2"/>
       <c r="V15" s="2"/>
-      <c r="W15" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="X15" s="2"/>
+      <c r="W15" s="2"/>
+      <c r="X15" s="2" t="s">
+        <v>36</v>
+      </c>
       <c r="Y15" s="2"/>
-      <c r="Z15" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="AA15" s="2"/>
+      <c r="Z15" s="2"/>
+      <c r="AA15" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="AB15" s="2"/>
       <c r="AC15" s="2"/>
-    </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD15" s="2"/>
+    </row>
+    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>118</v>
       </c>
@@ -2354,25 +2353,26 @@
       <c r="P16" s="2"/>
       <c r="Q16" s="2"/>
       <c r="R16" s="2"/>
-      <c r="S16" s="2" t="s">
+      <c r="S16" s="2"/>
+      <c r="T16" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="T16" s="2"/>
       <c r="U16" s="2"/>
       <c r="V16" s="2"/>
-      <c r="W16" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="X16" s="2"/>
+      <c r="W16" s="2"/>
+      <c r="X16" s="2" t="s">
+        <v>36</v>
+      </c>
       <c r="Y16" s="2"/>
-      <c r="Z16" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="AA16" s="2"/>
+      <c r="Z16" s="2"/>
+      <c r="AA16" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="AB16" s="2"/>
       <c r="AC16" s="2"/>
-    </row>
-    <row r="17" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD16" s="2"/>
+    </row>
+    <row r="17" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>123</v>
       </c>
@@ -2394,26 +2394,26 @@
       <c r="I17" t="s">
         <v>57</v>
       </c>
-      <c r="P17" t="s">
+      <c r="Q17" t="s">
         <v>129</v>
       </c>
-      <c r="R17" t="s">
+      <c r="S17" t="s">
         <v>130</v>
       </c>
-      <c r="S17" t="s">
+      <c r="T17" t="s">
         <v>131</v>
       </c>
-      <c r="U17" t="s">
+      <c r="V17" t="s">
         <v>132</v>
       </c>
-      <c r="W17" t="s">
-        <v>36</v>
-      </c>
-      <c r="Z17" t="s">
+      <c r="X17" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA17" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="18" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>134</v>
       </c>
@@ -2445,28 +2445,29 @@
       <c r="O18" s="2"/>
       <c r="P18" s="2"/>
       <c r="Q18" s="2"/>
-      <c r="R18" s="2" t="s">
+      <c r="R18" s="2"/>
+      <c r="S18" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="S18" s="2" t="s">
+      <c r="T18" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="T18" s="2"/>
       <c r="U18" s="2"/>
       <c r="V18" s="2"/>
-      <c r="W18" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="X18" s="2"/>
+      <c r="W18" s="2"/>
+      <c r="X18" s="2" t="s">
+        <v>36</v>
+      </c>
       <c r="Y18" s="2"/>
-      <c r="Z18" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="AA18" s="2"/>
+      <c r="Z18" s="2"/>
+      <c r="AA18" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="AB18" s="2"/>
       <c r="AC18" s="2"/>
-    </row>
-    <row r="19" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD18" s="2"/>
+    </row>
+    <row r="19" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>141</v>
       </c>
@@ -2498,30 +2499,31 @@
       <c r="O19" s="2"/>
       <c r="P19" s="2"/>
       <c r="Q19" s="2"/>
-      <c r="R19" s="2" t="s">
+      <c r="R19" s="2"/>
+      <c r="S19" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="S19" s="2" t="s">
+      <c r="T19" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="T19" s="2"/>
       <c r="U19" s="2"/>
       <c r="V19" s="2"/>
-      <c r="W19" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="X19" s="2"/>
-      <c r="Y19" s="2" t="s">
+      <c r="W19" s="2"/>
+      <c r="X19" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y19" s="2"/>
+      <c r="Z19" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="Z19" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="AA19" s="2"/>
+      <c r="AA19" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="AB19" s="2"/>
       <c r="AC19" s="2"/>
-    </row>
-    <row r="20" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD19" s="2"/>
+    </row>
+    <row r="20" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>148</v>
       </c>
@@ -2543,17 +2545,17 @@
       <c r="I20" t="s">
         <v>57</v>
       </c>
-      <c r="W20">
+      <c r="X20">
         <v>0</v>
       </c>
-      <c r="Y20" t="s">
+      <c r="Z20" t="s">
         <v>44</v>
       </c>
-      <c r="Z20" t="s">
+      <c r="AA20" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="21" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>152</v>
       </c>
@@ -2590,21 +2592,22 @@
       <c r="T21" s="2"/>
       <c r="U21" s="2"/>
       <c r="V21" s="2"/>
-      <c r="W21" s="2">
+      <c r="W21" s="2"/>
+      <c r="X21" s="2">
         <v>0</v>
       </c>
-      <c r="X21" s="2"/>
-      <c r="Y21" s="2" t="s">
+      <c r="Y21" s="2"/>
+      <c r="Z21" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="Z21" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="AA21" s="2"/>
+      <c r="AA21" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="AB21" s="2"/>
       <c r="AC21" s="2"/>
-    </row>
-    <row r="22" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD21" s="2"/>
+    </row>
+    <row r="22" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>156</v>
       </c>
@@ -2636,26 +2639,27 @@
       <c r="O22" s="2"/>
       <c r="P22" s="2"/>
       <c r="Q22" s="2"/>
-      <c r="R22" s="2" t="s">
+      <c r="R22" s="2"/>
+      <c r="S22" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="S22" s="2"/>
       <c r="T22" s="2"/>
       <c r="U22" s="2"/>
       <c r="V22" s="2"/>
-      <c r="W22" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="X22" s="2"/>
+      <c r="W22" s="2"/>
+      <c r="X22" s="2" t="s">
+        <v>36</v>
+      </c>
       <c r="Y22" s="2"/>
-      <c r="Z22" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="AA22" s="2"/>
+      <c r="Z22" s="2"/>
+      <c r="AA22" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="AB22" s="2"/>
       <c r="AC22" s="2"/>
-    </row>
-    <row r="23" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD22" s="2"/>
+    </row>
+    <row r="23" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>161</v>
       </c>
@@ -2687,30 +2691,31 @@
       <c r="O23" s="2"/>
       <c r="P23" s="2"/>
       <c r="Q23" s="2"/>
-      <c r="R23" s="2" t="s">
+      <c r="R23" s="2"/>
+      <c r="S23" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="S23" s="2" t="s">
+      <c r="T23" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="T23" s="2"/>
-      <c r="U23" s="2" t="s">
+      <c r="U23" s="2"/>
+      <c r="V23" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="V23" s="2"/>
-      <c r="W23" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="X23" s="2"/>
+      <c r="W23" s="2"/>
+      <c r="X23" s="2" t="s">
+        <v>36</v>
+      </c>
       <c r="Y23" s="2"/>
-      <c r="Z23" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="AA23" s="2"/>
+      <c r="Z23" s="2"/>
+      <c r="AA23" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="AB23" s="2"/>
       <c r="AC23" s="2"/>
-    </row>
-    <row r="24" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD23" s="2"/>
+    </row>
+    <row r="24" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>167</v>
       </c>
@@ -2732,20 +2737,20 @@
       <c r="I24" t="s">
         <v>57</v>
       </c>
-      <c r="R24" t="s">
+      <c r="S24" t="s">
         <v>172</v>
       </c>
-      <c r="W24" t="s">
-        <v>36</v>
-      </c>
-      <c r="Y24" t="s">
+      <c r="X24" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z24" t="s">
         <v>44</v>
       </c>
-      <c r="Z24" t="s">
+      <c r="AA24" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="25" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>173</v>
       </c>
@@ -2777,28 +2782,29 @@
       <c r="O25" s="2"/>
       <c r="P25" s="2"/>
       <c r="Q25" s="2"/>
-      <c r="R25" s="2" t="s">
+      <c r="R25" s="2"/>
+      <c r="S25" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="S25" s="2"/>
       <c r="T25" s="2"/>
       <c r="U25" s="2"/>
       <c r="V25" s="2"/>
-      <c r="W25" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="X25" s="2"/>
-      <c r="Y25" s="2" t="s">
+      <c r="W25" s="2"/>
+      <c r="X25" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y25" s="2"/>
+      <c r="Z25" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="Z25" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="AA25" s="2"/>
+      <c r="AA25" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="AB25" s="2"/>
       <c r="AC25" s="2"/>
-    </row>
-    <row r="26" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD25" s="2"/>
+    </row>
+    <row r="26" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>177</v>
       </c>
@@ -2830,30 +2836,31 @@
       <c r="O26" s="2"/>
       <c r="P26" s="2"/>
       <c r="Q26" s="2"/>
-      <c r="R26" s="2" t="s">
+      <c r="R26" s="2"/>
+      <c r="S26" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="S26" s="2" t="s">
+      <c r="T26" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="T26" s="2"/>
-      <c r="U26" s="2" t="s">
+      <c r="U26" s="2"/>
+      <c r="V26" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="V26" s="2"/>
-      <c r="W26" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="X26" s="2"/>
+      <c r="W26" s="2"/>
+      <c r="X26" s="2" t="s">
+        <v>36</v>
+      </c>
       <c r="Y26" s="2"/>
-      <c r="Z26" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="AA26" s="2"/>
+      <c r="Z26" s="2"/>
+      <c r="AA26" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="AB26" s="2"/>
       <c r="AC26" s="2"/>
-    </row>
-    <row r="27" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD26" s="2"/>
+    </row>
+    <row r="27" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>183</v>
       </c>
@@ -2885,30 +2892,31 @@
       <c r="O27" s="2"/>
       <c r="P27" s="2"/>
       <c r="Q27" s="2"/>
-      <c r="R27" s="2" t="s">
+      <c r="R27" s="2"/>
+      <c r="S27" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="S27" s="2" t="s">
+      <c r="T27" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="T27" s="2"/>
-      <c r="U27" s="2" t="s">
+      <c r="U27" s="2"/>
+      <c r="V27" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="V27" s="2"/>
-      <c r="W27" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="X27" s="2"/>
+      <c r="W27" s="2"/>
+      <c r="X27" s="2" t="s">
+        <v>36</v>
+      </c>
       <c r="Y27" s="2"/>
-      <c r="Z27" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="AA27" s="2"/>
+      <c r="Z27" s="2"/>
+      <c r="AA27" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="AB27" s="2"/>
       <c r="AC27" s="2"/>
-    </row>
-    <row r="28" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD27" s="2"/>
+    </row>
+    <row r="28" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>189</v>
       </c>
@@ -2940,30 +2948,31 @@
       <c r="O28" s="2"/>
       <c r="P28" s="2"/>
       <c r="Q28" s="2"/>
-      <c r="R28" s="2" t="s">
+      <c r="R28" s="2"/>
+      <c r="S28" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="S28" s="2" t="s">
+      <c r="T28" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="T28" s="2"/>
-      <c r="U28" s="2" t="s">
+      <c r="U28" s="2"/>
+      <c r="V28" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="V28" s="2"/>
-      <c r="W28" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="X28" s="2"/>
+      <c r="W28" s="2"/>
+      <c r="X28" s="2" t="s">
+        <v>36</v>
+      </c>
       <c r="Y28" s="2"/>
-      <c r="Z28" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="AA28" s="2"/>
+      <c r="Z28" s="2"/>
+      <c r="AA28" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="AB28" s="2"/>
       <c r="AC28" s="2"/>
-    </row>
-    <row r="29" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD28" s="2"/>
+    </row>
+    <row r="29" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>195</v>
       </c>
@@ -3000,21 +3009,22 @@
       <c r="T29" s="2"/>
       <c r="U29" s="2"/>
       <c r="V29" s="2"/>
-      <c r="W29" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="X29" s="2"/>
-      <c r="Y29" s="2" t="s">
+      <c r="W29" s="2"/>
+      <c r="X29" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y29" s="2"/>
+      <c r="Z29" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="Z29" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="AA29" s="2"/>
+      <c r="AA29" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="AB29" s="2"/>
       <c r="AC29" s="2"/>
-    </row>
-    <row r="30" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD29" s="2"/>
+    </row>
+    <row r="30" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>199</v>
       </c>
@@ -3046,30 +3056,31 @@
       <c r="O30" s="2"/>
       <c r="P30" s="2"/>
       <c r="Q30" s="2"/>
-      <c r="R30" s="2" t="s">
+      <c r="R30" s="2"/>
+      <c r="S30" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="S30" s="2" t="s">
+      <c r="T30" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="T30" s="2"/>
-      <c r="U30" s="2" t="s">
+      <c r="U30" s="2"/>
+      <c r="V30" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="V30" s="2"/>
-      <c r="W30" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="X30" s="2"/>
+      <c r="W30" s="2"/>
+      <c r="X30" s="2" t="s">
+        <v>36</v>
+      </c>
       <c r="Y30" s="2"/>
-      <c r="Z30" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="AA30" s="2"/>
+      <c r="Z30" s="2"/>
+      <c r="AA30" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="AB30" s="2"/>
       <c r="AC30" s="2"/>
-    </row>
-    <row r="31" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD30" s="2"/>
+    </row>
+    <row r="31" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>205</v>
       </c>
@@ -3101,30 +3112,31 @@
       <c r="O31" s="2"/>
       <c r="P31" s="2"/>
       <c r="Q31" s="2"/>
-      <c r="R31" s="2" t="s">
+      <c r="R31" s="2"/>
+      <c r="S31" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="S31" s="2" t="s">
+      <c r="T31" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="T31" s="2"/>
-      <c r="U31" s="2" t="s">
+      <c r="U31" s="2"/>
+      <c r="V31" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="V31" s="2"/>
-      <c r="W31" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="X31" s="2"/>
+      <c r="W31" s="2"/>
+      <c r="X31" s="2" t="s">
+        <v>36</v>
+      </c>
       <c r="Y31" s="2"/>
-      <c r="Z31" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="AA31" s="2"/>
+      <c r="Z31" s="2"/>
+      <c r="AA31" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="AB31" s="2"/>
       <c r="AC31" s="2"/>
-    </row>
-    <row r="32" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD31" s="2"/>
+    </row>
+    <row r="32" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>211</v>
       </c>
@@ -3158,30 +3170,31 @@
       <c r="O32" s="2"/>
       <c r="P32" s="2"/>
       <c r="Q32" s="2"/>
-      <c r="R32" s="2" t="s">
+      <c r="R32" s="2"/>
+      <c r="S32" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="S32" s="2" t="s">
+      <c r="T32" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="T32" s="2"/>
       <c r="U32" s="2"/>
       <c r="V32" s="2"/>
-      <c r="W32" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="X32" s="2"/>
-      <c r="Y32" s="2" t="s">
+      <c r="W32" s="2"/>
+      <c r="X32" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y32" s="2"/>
+      <c r="Z32" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="Z32" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="AA32" s="2"/>
+      <c r="AA32" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="AB32" s="2"/>
       <c r="AC32" s="2"/>
-    </row>
-    <row r="33" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD32" s="2"/>
+    </row>
+    <row r="33" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>219</v>
       </c>
@@ -3213,183 +3226,186 @@
       <c r="O33" s="2"/>
       <c r="P33" s="2"/>
       <c r="Q33" s="2"/>
-      <c r="R33" s="2" t="s">
+      <c r="R33" s="2"/>
+      <c r="S33" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="S33" s="2" t="s">
+      <c r="T33" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="T33" s="2"/>
-      <c r="U33" s="2" t="s">
+      <c r="U33" s="2"/>
+      <c r="V33" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="V33" s="2"/>
-      <c r="W33" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="X33" s="2"/>
+      <c r="W33" s="2"/>
+      <c r="X33" s="2" t="s">
+        <v>36</v>
+      </c>
       <c r="Y33" s="2"/>
-      <c r="Z33" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="AA33" s="2"/>
+      <c r="Z33" s="2"/>
+      <c r="AA33" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="AB33" s="2"/>
       <c r="AC33" s="2"/>
-    </row>
-    <row r="34" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A34" s="3" t="s">
+      <c r="AD33" s="2"/>
+    </row>
+    <row r="34" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+      <c r="G34" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="I34" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="J34" s="2"/>
+      <c r="K34" s="2"/>
+      <c r="L34" s="2"/>
+      <c r="M34" s="2"/>
+      <c r="N34" s="2"/>
+      <c r="O34" s="2"/>
+      <c r="P34" s="2"/>
+      <c r="Q34" s="2"/>
+      <c r="R34" s="2"/>
+      <c r="S34" s="2"/>
+      <c r="T34" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="U34" s="2"/>
+      <c r="V34" s="2"/>
+      <c r="W34" s="2"/>
+      <c r="X34" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y34" s="2"/>
+      <c r="Z34" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="AA34" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="AB34" s="2"/>
+      <c r="AC34" s="2"/>
+      <c r="AD34" s="2"/>
+    </row>
+    <row r="35" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>230</v>
+      </c>
+      <c r="B35" t="s">
+        <v>176</v>
+      </c>
+      <c r="C35" t="s">
+        <v>231</v>
+      </c>
+      <c r="D35" t="s">
+        <v>232</v>
+      </c>
+      <c r="G35" t="s">
+        <v>32</v>
+      </c>
+      <c r="H35" t="s">
+        <v>32</v>
+      </c>
+      <c r="I35" t="s">
         <v>225</v>
       </c>
-      <c r="B34" s="3" t="s">
-        <v>226</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>227</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>228</v>
-      </c>
-      <c r="E34" s="3"/>
-      <c r="F34" s="3"/>
-      <c r="G34" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="H34" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="I34" s="3" t="s">
-        <v>229</v>
-      </c>
-      <c r="J34" s="3"/>
-      <c r="K34" s="3"/>
-      <c r="L34" s="3"/>
-      <c r="M34" s="3"/>
-      <c r="N34" s="3"/>
-      <c r="O34" s="3"/>
-      <c r="P34" s="3"/>
-      <c r="Q34" s="3"/>
-      <c r="R34" s="3"/>
-      <c r="S34" s="3"/>
-      <c r="T34" s="3"/>
-      <c r="U34" s="3"/>
-      <c r="V34" s="3"/>
-      <c r="W34" s="3"/>
-      <c r="X34" s="3"/>
-      <c r="Y34" s="3" t="s">
+      <c r="Z35" t="s">
         <v>44</v>
       </c>
-      <c r="Z34" s="3" t="s">
-        <v>230</v>
-      </c>
-      <c r="AA34" s="3"/>
-      <c r="AB34" s="3"/>
-      <c r="AC34" s="3"/>
-    </row>
-    <row r="35" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
-        <v>231</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="C35" s="2" t="s">
+      <c r="AA35" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="36" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="D35" s="2" t="s">
+      <c r="B36" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C36" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="E35" s="2"/>
-      <c r="F35" s="2"/>
-      <c r="G35" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="H35" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="I35" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="J35" s="2"/>
-      <c r="K35" s="2"/>
-      <c r="L35" s="2"/>
-      <c r="M35" s="2"/>
-      <c r="N35" s="2"/>
-      <c r="O35" s="2"/>
-      <c r="P35" s="2"/>
-      <c r="Q35" s="2"/>
-      <c r="R35" s="2"/>
-      <c r="S35" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="T35" s="2"/>
-      <c r="U35" s="2"/>
-      <c r="V35" s="2"/>
-      <c r="W35" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="X35" s="2"/>
-      <c r="Y35" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="Z35" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="AA35" s="2"/>
-      <c r="AB35" s="2"/>
-      <c r="AC35" s="2"/>
-    </row>
-    <row r="36" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+      <c r="D36" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="B36" t="s">
-        <v>176</v>
-      </c>
-      <c r="C36" t="s">
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
+      <c r="G36" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="H36" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="I36" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="J36" s="2"/>
+      <c r="K36" s="2"/>
+      <c r="L36" s="2"/>
+      <c r="M36" s="2"/>
+      <c r="N36" s="2"/>
+      <c r="O36" s="2"/>
+      <c r="P36" s="2"/>
+      <c r="Q36" s="2"/>
+      <c r="R36" s="2"/>
+      <c r="S36" s="2"/>
+      <c r="T36" s="2"/>
+      <c r="U36" s="2"/>
+      <c r="V36" s="2"/>
+      <c r="W36" s="2"/>
+      <c r="X36" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y36" s="2"/>
+      <c r="Z36" s="2"/>
+      <c r="AA36" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="AB36" s="2"/>
+      <c r="AC36" s="2"/>
+      <c r="AD36" s="2"/>
+    </row>
+    <row r="37" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="D36" t="s">
+      <c r="B37" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="G36" t="s">
-        <v>32</v>
-      </c>
-      <c r="H36" t="s">
-        <v>32</v>
-      </c>
-      <c r="I36" t="s">
-        <v>229</v>
-      </c>
-      <c r="Y36" t="s">
-        <v>44</v>
-      </c>
-      <c r="Z36" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="37" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
+      <c r="C37" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="B37" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="C37" s="2" t="s">
+      <c r="D37" s="2" t="s">
         <v>239</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>240</v>
       </c>
       <c r="E37" s="2"/>
       <c r="F37" s="2"/>
       <c r="G37" s="2" t="s">
-        <v>105</v>
+        <v>56</v>
       </c>
       <c r="H37" s="2" t="s">
         <v>56</v>
       </c>
       <c r="I37" s="2" t="s">
-        <v>33</v>
+        <v>225</v>
       </c>
       <c r="J37" s="2"/>
       <c r="K37" s="2"/>
@@ -3401,22 +3417,25 @@
       <c r="Q37" s="2"/>
       <c r="R37" s="2"/>
       <c r="S37" s="2"/>
-      <c r="T37" s="2"/>
+      <c r="T37" s="2" t="s">
+        <v>240</v>
+      </c>
       <c r="U37" s="2"/>
       <c r="V37" s="2"/>
-      <c r="W37" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="X37" s="2"/>
+      <c r="W37" s="2"/>
+      <c r="X37" s="2" t="s">
+        <v>36</v>
+      </c>
       <c r="Y37" s="2"/>
-      <c r="Z37" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="AA37" s="2"/>
+      <c r="Z37" s="2"/>
+      <c r="AA37" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="AB37" s="2"/>
       <c r="AC37" s="2"/>
-    </row>
-    <row r="38" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD37" s="2"/>
+    </row>
+    <row r="38" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>241</v>
       </c>
@@ -3432,13 +3451,13 @@
       <c r="E38" s="2"/>
       <c r="F38" s="2"/>
       <c r="G38" s="2" t="s">
-        <v>56</v>
+        <v>245</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>56</v>
+        <v>246</v>
       </c>
       <c r="I38" s="2" t="s">
-        <v>229</v>
+        <v>33</v>
       </c>
       <c r="J38" s="2"/>
       <c r="K38" s="2"/>
@@ -3450,114 +3469,120 @@
       <c r="Q38" s="2"/>
       <c r="R38" s="2"/>
       <c r="S38" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="T38" s="2"/>
+        <v>34</v>
+      </c>
+      <c r="T38" s="2" t="s">
+        <v>247</v>
+      </c>
       <c r="U38" s="2"/>
       <c r="V38" s="2"/>
-      <c r="W38" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="X38" s="2"/>
+      <c r="W38" s="2"/>
+      <c r="X38" s="2" t="s">
+        <v>36</v>
+      </c>
       <c r="Y38" s="2"/>
-      <c r="Z38" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="AA38" s="2"/>
+      <c r="Z38" s="2"/>
+      <c r="AA38" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="AB38" s="2"/>
       <c r="AC38" s="2"/>
-    </row>
-    <row r="39" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
-        <v>246</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="C39" s="2" t="s">
+      <c r="AD38" s="2"/>
+    </row>
+    <row r="39" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>248</v>
       </c>
-      <c r="D39" s="2" t="s">
+      <c r="B39" t="s">
+        <v>171</v>
+      </c>
+      <c r="C39" t="s">
         <v>249</v>
       </c>
-      <c r="E39" s="2"/>
-      <c r="F39" s="2"/>
-      <c r="G39" s="2" t="s">
+      <c r="D39" t="s">
         <v>250</v>
       </c>
-      <c r="H39" s="2" t="s">
+      <c r="G39" t="s">
+        <v>153</v>
+      </c>
+      <c r="H39" t="s">
+        <v>56</v>
+      </c>
+      <c r="I39" t="s">
+        <v>57</v>
+      </c>
+      <c r="S39" t="s">
         <v>251</v>
       </c>
-      <c r="I39" s="2" t="s">
+      <c r="X39" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA39" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="40" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="E40" s="2"/>
+      <c r="F40" s="2"/>
+      <c r="G40" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="H40" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="I40" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="J39" s="2"/>
-      <c r="K39" s="2"/>
-      <c r="L39" s="2"/>
-      <c r="M39" s="2"/>
-      <c r="N39" s="2"/>
-      <c r="O39" s="2"/>
-      <c r="P39" s="2"/>
-      <c r="Q39" s="2"/>
-      <c r="R39" s="2" t="s">
+      <c r="J40" s="2"/>
+      <c r="K40" s="2"/>
+      <c r="L40" s="2"/>
+      <c r="M40" s="2"/>
+      <c r="N40" s="2"/>
+      <c r="O40" s="2"/>
+      <c r="P40" s="2"/>
+      <c r="Q40" s="2"/>
+      <c r="R40" s="2"/>
+      <c r="S40" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="S39" s="2" t="s">
-        <v>252</v>
-      </c>
-      <c r="T39" s="2"/>
-      <c r="U39" s="2"/>
-      <c r="V39" s="2"/>
-      <c r="W39" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="X39" s="2"/>
-      <c r="Y39" s="2"/>
-      <c r="Z39" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="AA39" s="2"/>
-      <c r="AB39" s="2"/>
-      <c r="AC39" s="2"/>
-    </row>
-    <row r="40" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>253</v>
-      </c>
-      <c r="B40" t="s">
-        <v>171</v>
-      </c>
-      <c r="C40" t="s">
-        <v>254</v>
-      </c>
-      <c r="D40" t="s">
-        <v>255</v>
-      </c>
-      <c r="G40" t="s">
-        <v>153</v>
-      </c>
-      <c r="H40" t="s">
-        <v>56</v>
-      </c>
-      <c r="I40" t="s">
-        <v>57</v>
-      </c>
-      <c r="R40" t="s">
+      <c r="T40" s="2" t="s">
         <v>256</v>
       </c>
-      <c r="W40" t="s">
-        <v>36</v>
-      </c>
-      <c r="Z40" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="41" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="U40" s="2"/>
+      <c r="V40" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="W40" s="2"/>
+      <c r="X40" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y40" s="2"/>
+      <c r="Z40" s="2"/>
+      <c r="AA40" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="AB40" s="2"/>
+      <c r="AC40" s="2"/>
+      <c r="AD40" s="2"/>
+    </row>
+    <row r="41" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>258</v>
+        <v>55</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>259</v>
@@ -3568,13 +3593,13 @@
       <c r="E41" s="2"/>
       <c r="F41" s="2"/>
       <c r="G41" s="2" t="s">
-        <v>86</v>
+        <v>261</v>
       </c>
       <c r="H41" s="2" t="s">
         <v>56</v>
       </c>
       <c r="I41" s="2" t="s">
-        <v>33</v>
+        <v>57</v>
       </c>
       <c r="J41" s="2"/>
       <c r="K41" s="2"/>
@@ -3584,52 +3609,49 @@
       <c r="O41" s="2"/>
       <c r="P41" s="2"/>
       <c r="Q41" s="2"/>
-      <c r="R41" s="2" t="s">
-        <v>34</v>
-      </c>
+      <c r="R41" s="2"/>
       <c r="S41" s="2" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="T41" s="2"/>
-      <c r="U41" s="2" t="s">
-        <v>262</v>
-      </c>
+      <c r="U41" s="2"/>
       <c r="V41" s="2"/>
-      <c r="W41" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="X41" s="2"/>
+      <c r="W41" s="2"/>
+      <c r="X41" s="2" t="s">
+        <v>36</v>
+      </c>
       <c r="Y41" s="2"/>
-      <c r="Z41" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="AA41" s="2"/>
+      <c r="Z41" s="2"/>
+      <c r="AA41" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="AB41" s="2"/>
       <c r="AC41" s="2"/>
-    </row>
-    <row r="42" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD41" s="2"/>
+    </row>
+    <row r="42" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>263</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>55</v>
+        <v>264</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="E42" s="2"/>
       <c r="F42" s="2"/>
       <c r="G42" s="2" t="s">
-        <v>266</v>
+        <v>56</v>
       </c>
       <c r="H42" s="2" t="s">
         <v>56</v>
       </c>
       <c r="I42" s="2" t="s">
-        <v>57</v>
+        <v>33</v>
       </c>
       <c r="J42" s="2"/>
       <c r="K42" s="2"/>
@@ -3639,26 +3661,27 @@
       <c r="O42" s="2"/>
       <c r="P42" s="2"/>
       <c r="Q42" s="2"/>
-      <c r="R42" s="2" t="s">
+      <c r="R42" s="2"/>
+      <c r="S42" s="2" t="s">
         <v>267</v>
       </c>
-      <c r="S42" s="2"/>
       <c r="T42" s="2"/>
       <c r="U42" s="2"/>
       <c r="V42" s="2"/>
-      <c r="W42" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="X42" s="2"/>
+      <c r="W42" s="2"/>
+      <c r="X42" s="2" t="s">
+        <v>36</v>
+      </c>
       <c r="Y42" s="2"/>
-      <c r="Z42" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="AA42" s="2"/>
+      <c r="Z42" s="2"/>
+      <c r="AA42" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="AB42" s="2"/>
       <c r="AC42" s="2"/>
-    </row>
-    <row r="43" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD42" s="2"/>
+    </row>
+    <row r="43" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>268</v>
       </c>
@@ -3672,15 +3695,17 @@
         <v>271</v>
       </c>
       <c r="E43" s="2"/>
-      <c r="F43" s="2"/>
+      <c r="F43" s="2" t="s">
+        <v>272</v>
+      </c>
       <c r="G43" s="2" t="s">
-        <v>56</v>
+        <v>212</v>
       </c>
       <c r="H43" s="2" t="s">
         <v>56</v>
       </c>
       <c r="I43" s="2" t="s">
-        <v>33</v>
+        <v>225</v>
       </c>
       <c r="J43" s="2"/>
       <c r="K43" s="2"/>
@@ -3690,50 +3715,49 @@
       <c r="O43" s="2"/>
       <c r="P43" s="2"/>
       <c r="Q43" s="2"/>
-      <c r="R43" s="2" t="s">
-        <v>272</v>
-      </c>
+      <c r="R43" s="2"/>
       <c r="S43" s="2"/>
       <c r="T43" s="2"/>
       <c r="U43" s="2"/>
       <c r="V43" s="2"/>
-      <c r="W43" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="X43" s="2"/>
+      <c r="W43" s="2"/>
+      <c r="X43" s="2" t="s">
+        <v>36</v>
+      </c>
       <c r="Y43" s="2"/>
       <c r="Z43" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="AA43" s="2"/>
+        <v>44</v>
+      </c>
+      <c r="AA43" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="AB43" s="2"/>
       <c r="AC43" s="2"/>
-    </row>
-    <row r="44" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD43" s="2"/>
+    </row>
+    <row r="44" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>273</v>
       </c>
       <c r="B44" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="C44" s="2" t="s">
         <v>274</v>
       </c>
-      <c r="C44" s="2" t="s">
+      <c r="D44" s="2" t="s">
         <v>275</v>
       </c>
-      <c r="D44" s="2" t="s">
-        <v>276</v>
-      </c>
       <c r="E44" s="2"/>
-      <c r="F44" s="2" t="s">
-        <v>277</v>
-      </c>
+      <c r="F44" s="2"/>
       <c r="G44" s="2" t="s">
-        <v>212</v>
+        <v>149</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>56</v>
+        <v>128</v>
       </c>
       <c r="I44" s="2" t="s">
-        <v>229</v>
+        <v>57</v>
       </c>
       <c r="J44" s="2"/>
       <c r="K44" s="2"/>
@@ -3748,43 +3772,44 @@
       <c r="T44" s="2"/>
       <c r="U44" s="2"/>
       <c r="V44" s="2"/>
-      <c r="W44" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="X44" s="2"/>
-      <c r="Y44" s="2" t="s">
+      <c r="W44" s="2"/>
+      <c r="X44" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y44" s="2"/>
+      <c r="Z44" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="Z44" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="AA44" s="2"/>
+      <c r="AA44" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="AB44" s="2"/>
       <c r="AC44" s="2"/>
-    </row>
-    <row r="45" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD44" s="2"/>
+    </row>
+    <row r="45" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="C45" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="B45" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="C45" s="2" t="s">
+      <c r="D45" s="2" t="s">
         <v>279</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>280</v>
       </c>
       <c r="E45" s="2"/>
       <c r="F45" s="2"/>
       <c r="G45" s="2" t="s">
-        <v>149</v>
+        <v>86</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>128</v>
+        <v>56</v>
       </c>
       <c r="I45" s="2" t="s">
-        <v>57</v>
+        <v>33</v>
       </c>
       <c r="J45" s="2"/>
       <c r="K45" s="2"/>
@@ -3795,25 +3820,28 @@
       <c r="P45" s="2"/>
       <c r="Q45" s="2"/>
       <c r="R45" s="2"/>
-      <c r="S45" s="2"/>
-      <c r="T45" s="2"/>
+      <c r="S45" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="T45" s="2" t="s">
+        <v>280</v>
+      </c>
       <c r="U45" s="2"/>
       <c r="V45" s="2"/>
-      <c r="W45" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="X45" s="2"/>
-      <c r="Y45" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="Z45" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="AA45" s="2"/>
+      <c r="W45" s="2"/>
+      <c r="X45" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y45" s="2"/>
+      <c r="Z45" s="2"/>
+      <c r="AA45" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="AB45" s="2"/>
       <c r="AC45" s="2"/>
-    </row>
-    <row r="46" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD45" s="2"/>
+    </row>
+    <row r="46" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>281</v>
       </c>
@@ -3829,13 +3857,13 @@
       <c r="E46" s="2"/>
       <c r="F46" s="2"/>
       <c r="G46" s="2" t="s">
-        <v>86</v>
+        <v>124</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>56</v>
+        <v>128</v>
       </c>
       <c r="I46" s="2" t="s">
-        <v>33</v>
+        <v>57</v>
       </c>
       <c r="J46" s="2"/>
       <c r="K46" s="2"/>
@@ -3845,44 +3873,45 @@
       <c r="O46" s="2"/>
       <c r="P46" s="2"/>
       <c r="Q46" s="2"/>
-      <c r="R46" s="2" t="s">
-        <v>34</v>
-      </c>
+      <c r="R46" s="2"/>
       <c r="S46" s="2" t="s">
         <v>285</v>
       </c>
       <c r="T46" s="2"/>
       <c r="U46" s="2"/>
-      <c r="V46" s="2"/>
-      <c r="W46" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="X46" s="2"/>
+      <c r="V46" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="W46" s="2"/>
+      <c r="X46" s="2" t="s">
+        <v>36</v>
+      </c>
       <c r="Y46" s="2"/>
-      <c r="Z46" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="AA46" s="2"/>
+      <c r="Z46" s="2"/>
+      <c r="AA46" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="AB46" s="2"/>
       <c r="AC46" s="2"/>
-    </row>
-    <row r="47" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD46" s="2"/>
+    </row>
+    <row r="47" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="E47" s="2"/>
       <c r="F47" s="2"/>
       <c r="G47" s="2" t="s">
-        <v>124</v>
+        <v>142</v>
       </c>
       <c r="H47" s="2" t="s">
         <v>128</v>
@@ -3898,50 +3927,53 @@
       <c r="O47" s="2"/>
       <c r="P47" s="2"/>
       <c r="Q47" s="2"/>
-      <c r="R47" s="2" t="s">
-        <v>290</v>
-      </c>
-      <c r="S47" s="2"/>
+      <c r="R47" s="2"/>
+      <c r="S47" s="2" t="s">
+        <v>291</v>
+      </c>
       <c r="T47" s="2"/>
-      <c r="U47" s="2" t="s">
-        <v>291</v>
-      </c>
-      <c r="V47" s="2"/>
-      <c r="W47" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="X47" s="2"/>
+      <c r="U47" s="2"/>
+      <c r="V47" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="W47" s="2"/>
+      <c r="X47" s="2" t="s">
+        <v>36</v>
+      </c>
       <c r="Y47" s="2"/>
       <c r="Z47" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="AA47" s="2"/>
+        <v>44</v>
+      </c>
+      <c r="AA47" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="AB47" s="2"/>
       <c r="AC47" s="2"/>
-    </row>
-    <row r="48" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD47" s="2"/>
+    </row>
+    <row r="48" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="E48" s="2"/>
       <c r="F48" s="2"/>
       <c r="G48" s="2" t="s">
-        <v>142</v>
+        <v>56</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>128</v>
+        <v>56</v>
       </c>
       <c r="I48" s="2" t="s">
-        <v>57</v>
+        <v>216</v>
       </c>
       <c r="J48" s="2"/>
       <c r="K48" s="2"/>
@@ -3951,41 +3983,42 @@
       <c r="O48" s="2"/>
       <c r="P48" s="2"/>
       <c r="Q48" s="2"/>
-      <c r="R48" s="2" t="s">
-        <v>296</v>
-      </c>
-      <c r="S48" s="2"/>
+      <c r="R48" s="2"/>
+      <c r="S48" s="2" t="s">
+        <v>297</v>
+      </c>
       <c r="T48" s="2"/>
-      <c r="U48" s="2" t="s">
-        <v>297</v>
-      </c>
+      <c r="U48" s="2"/>
       <c r="V48" s="2"/>
-      <c r="W48" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="X48" s="2"/>
-      <c r="Y48" s="2" t="s">
+      <c r="W48" s="2"/>
+      <c r="X48" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y48" s="2"/>
+      <c r="Z48" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="Z48" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="AA48" s="2"/>
+      <c r="AA48" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="AB48" s="2"/>
       <c r="AC48" s="2"/>
-    </row>
-    <row r="49" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD48" s="2" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="49" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="E49" s="2"/>
       <c r="F49" s="2"/>
@@ -3996,7 +4029,7 @@
         <v>56</v>
       </c>
       <c r="I49" s="2" t="s">
-        <v>216</v>
+        <v>33</v>
       </c>
       <c r="J49" s="2"/>
       <c r="K49" s="2"/>
@@ -4006,49 +4039,46 @@
       <c r="O49" s="2"/>
       <c r="P49" s="2"/>
       <c r="Q49" s="2"/>
-      <c r="R49" s="2" t="s">
-        <v>302</v>
-      </c>
-      <c r="S49" s="2"/>
+      <c r="R49" s="2"/>
+      <c r="S49" s="2" t="s">
+        <v>267</v>
+      </c>
       <c r="T49" s="2"/>
       <c r="U49" s="2"/>
       <c r="V49" s="2"/>
-      <c r="W49" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="X49" s="2"/>
-      <c r="Y49" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="Z49" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="AA49" s="2"/>
+      <c r="W49" s="2"/>
+      <c r="X49" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y49" s="2"/>
+      <c r="Z49" s="2"/>
+      <c r="AA49" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="AB49" s="2"/>
-      <c r="AC49" s="2" t="s">
+      <c r="AC49" s="2"/>
+      <c r="AD49" s="2"/>
+    </row>
+    <row r="50" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="50" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A50" s="2" t="s">
+      <c r="B50" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="B50" s="2" t="s">
+      <c r="C50" s="2" t="s">
         <v>305</v>
       </c>
-      <c r="C50" s="2" t="s">
+      <c r="D50" s="2" t="s">
         <v>306</v>
-      </c>
-      <c r="D50" s="2" t="s">
-        <v>307</v>
       </c>
       <c r="E50" s="2"/>
       <c r="F50" s="2"/>
       <c r="G50" s="2" t="s">
-        <v>56</v>
+        <v>28</v>
       </c>
       <c r="H50" s="2" t="s">
-        <v>56</v>
+        <v>32</v>
       </c>
       <c r="I50" s="2" t="s">
         <v>33</v>
@@ -4061,48 +4091,53 @@
       <c r="O50" s="2"/>
       <c r="P50" s="2"/>
       <c r="Q50" s="2"/>
-      <c r="R50" s="2" t="s">
-        <v>272</v>
-      </c>
-      <c r="S50" s="2"/>
-      <c r="T50" s="2"/>
+      <c r="R50" s="2"/>
+      <c r="S50" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="T50" s="2" t="s">
+        <v>307</v>
+      </c>
       <c r="U50" s="2"/>
-      <c r="V50" s="2"/>
-      <c r="W50" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="X50" s="2"/>
+      <c r="V50" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="W50" s="2"/>
+      <c r="X50" s="2" t="s">
+        <v>36</v>
+      </c>
       <c r="Y50" s="2"/>
-      <c r="Z50" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="AA50" s="2"/>
+      <c r="Z50" s="2"/>
+      <c r="AA50" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="AB50" s="2"/>
       <c r="AC50" s="2"/>
-    </row>
-    <row r="51" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD50" s="2"/>
+    </row>
+    <row r="51" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="E51" s="2"/>
       <c r="F51" s="2"/>
       <c r="G51" s="2" t="s">
-        <v>28</v>
+        <v>124</v>
       </c>
       <c r="H51" s="2" t="s">
-        <v>32</v>
+        <v>128</v>
       </c>
       <c r="I51" s="2" t="s">
-        <v>33</v>
+        <v>57</v>
       </c>
       <c r="J51" s="2"/>
       <c r="K51" s="2"/>
@@ -4112,35 +4147,34 @@
       <c r="O51" s="2"/>
       <c r="P51" s="2"/>
       <c r="Q51" s="2"/>
-      <c r="R51" s="2" t="s">
-        <v>34</v>
-      </c>
+      <c r="R51" s="2"/>
       <c r="S51" s="2" t="s">
-        <v>312</v>
-      </c>
-      <c r="T51" s="2"/>
-      <c r="U51" s="2" t="s">
         <v>313</v>
       </c>
+      <c r="T51" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="U51" s="2"/>
       <c r="V51" s="2"/>
-      <c r="W51" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="X51" s="2"/>
+      <c r="W51" s="2"/>
+      <c r="X51" s="2" t="s">
+        <v>36</v>
+      </c>
       <c r="Y51" s="2"/>
-      <c r="Z51" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="AA51" s="2"/>
+      <c r="Z51" s="2"/>
+      <c r="AA51" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="AB51" s="2"/>
       <c r="AC51" s="2"/>
-    </row>
-    <row r="52" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD51" s="2"/>
+    </row>
+    <row r="52" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>315</v>
+        <v>261</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>316</v>
@@ -4151,10 +4185,10 @@
       <c r="E52" s="2"/>
       <c r="F52" s="2"/>
       <c r="G52" s="2" t="s">
-        <v>124</v>
+        <v>157</v>
       </c>
       <c r="H52" s="2" t="s">
-        <v>128</v>
+        <v>56</v>
       </c>
       <c r="I52" s="2" t="s">
         <v>57</v>
@@ -4167,44 +4201,43 @@
       <c r="O52" s="2"/>
       <c r="P52" s="2"/>
       <c r="Q52" s="2"/>
-      <c r="R52" s="2" t="s">
-        <v>318</v>
-      </c>
+      <c r="R52" s="2"/>
       <c r="S52" s="2" t="s">
-        <v>319</v>
+        <v>160</v>
       </c>
       <c r="T52" s="2"/>
       <c r="U52" s="2"/>
       <c r="V52" s="2"/>
-      <c r="W52" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="X52" s="2"/>
+      <c r="W52" s="2"/>
+      <c r="X52" s="2" t="s">
+        <v>36</v>
+      </c>
       <c r="Y52" s="2"/>
-      <c r="Z52" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="AA52" s="2"/>
+      <c r="Z52" s="2"/>
+      <c r="AA52" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="AB52" s="2"/>
       <c r="AC52" s="2"/>
-    </row>
-    <row r="53" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD52" s="2"/>
+    </row>
+    <row r="53" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="C53" s="2" t="s">
         <v>320</v>
       </c>
-      <c r="B53" s="2" t="s">
-        <v>266</v>
-      </c>
-      <c r="C53" s="2" t="s">
+      <c r="D53" s="2" t="s">
         <v>321</v>
-      </c>
-      <c r="D53" s="2" t="s">
-        <v>322</v>
       </c>
       <c r="E53" s="2"/>
       <c r="F53" s="2"/>
       <c r="G53" s="2" t="s">
-        <v>157</v>
+        <v>55</v>
       </c>
       <c r="H53" s="2" t="s">
         <v>56</v>
@@ -4220,42 +4253,45 @@
       <c r="O53" s="2"/>
       <c r="P53" s="2"/>
       <c r="Q53" s="2"/>
-      <c r="R53" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="S53" s="2"/>
+      <c r="R53" s="2"/>
+      <c r="S53" s="2" t="s">
+        <v>322</v>
+      </c>
       <c r="T53" s="2"/>
       <c r="U53" s="2"/>
-      <c r="V53" s="2"/>
-      <c r="W53" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="X53" s="2"/>
+      <c r="V53" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="W53" s="2"/>
+      <c r="X53" s="2" t="s">
+        <v>36</v>
+      </c>
       <c r="Y53" s="2"/>
-      <c r="Z53" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="AA53" s="2"/>
+      <c r="Z53" s="2"/>
+      <c r="AA53" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="AB53" s="2"/>
       <c r="AC53" s="2"/>
-    </row>
-    <row r="54" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD53" s="2"/>
+    </row>
+    <row r="54" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="E54" s="2"/>
       <c r="F54" s="2"/>
       <c r="G54" s="2" t="s">
-        <v>55</v>
+        <v>328</v>
       </c>
       <c r="H54" s="2" t="s">
         <v>56</v>
@@ -4271,50 +4307,49 @@
       <c r="O54" s="2"/>
       <c r="P54" s="2"/>
       <c r="Q54" s="2"/>
-      <c r="R54" s="2" t="s">
-        <v>327</v>
-      </c>
-      <c r="S54" s="2"/>
+      <c r="R54" s="2"/>
+      <c r="S54" s="2" t="s">
+        <v>329</v>
+      </c>
       <c r="T54" s="2"/>
-      <c r="U54" s="2" t="s">
-        <v>328</v>
-      </c>
+      <c r="U54" s="2"/>
       <c r="V54" s="2"/>
-      <c r="W54" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="X54" s="2"/>
+      <c r="W54" s="2"/>
+      <c r="X54" s="2" t="s">
+        <v>36</v>
+      </c>
       <c r="Y54" s="2"/>
-      <c r="Z54" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="AA54" s="2"/>
+      <c r="Z54" s="2"/>
+      <c r="AA54" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="AB54" s="2"/>
       <c r="AC54" s="2"/>
-    </row>
-    <row r="55" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD54" s="2"/>
+    </row>
+    <row r="55" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="E55" s="2"/>
       <c r="F55" s="2"/>
       <c r="G55" s="2" t="s">
-        <v>333</v>
+        <v>86</v>
       </c>
       <c r="H55" s="2" t="s">
         <v>56</v>
       </c>
       <c r="I55" s="2" t="s">
-        <v>57</v>
+        <v>33</v>
       </c>
       <c r="J55" s="2"/>
       <c r="K55" s="2"/>
@@ -4324,48 +4359,53 @@
       <c r="O55" s="2"/>
       <c r="P55" s="2"/>
       <c r="Q55" s="2"/>
-      <c r="R55" s="2" t="s">
+      <c r="R55" s="2"/>
+      <c r="S55" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="T55" s="2" t="s">
         <v>334</v>
       </c>
-      <c r="S55" s="2"/>
-      <c r="T55" s="2"/>
       <c r="U55" s="2"/>
-      <c r="V55" s="2"/>
-      <c r="W55" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="X55" s="2"/>
+      <c r="V55" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="W55" s="2"/>
+      <c r="X55" s="2" t="s">
+        <v>36</v>
+      </c>
       <c r="Y55" s="2"/>
-      <c r="Z55" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="AA55" s="2"/>
+      <c r="Z55" s="2"/>
+      <c r="AA55" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="AB55" s="2"/>
       <c r="AC55" s="2"/>
-    </row>
-    <row r="56" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD55" s="2"/>
+    </row>
+    <row r="56" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="E56" s="2"/>
       <c r="F56" s="2"/>
       <c r="G56" s="2" t="s">
-        <v>86</v>
+        <v>142</v>
       </c>
       <c r="H56" s="2" t="s">
-        <v>56</v>
+        <v>128</v>
       </c>
       <c r="I56" s="2" t="s">
-        <v>33</v>
+        <v>57</v>
       </c>
       <c r="J56" s="2"/>
       <c r="K56" s="2"/>
@@ -4375,30 +4415,29 @@
       <c r="O56" s="2"/>
       <c r="P56" s="2"/>
       <c r="Q56" s="2"/>
-      <c r="R56" s="2" t="s">
-        <v>34</v>
-      </c>
+      <c r="R56" s="2"/>
       <c r="S56" s="2" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="T56" s="2"/>
-      <c r="U56" s="2" t="s">
-        <v>340</v>
-      </c>
+      <c r="U56" s="2"/>
       <c r="V56" s="2"/>
-      <c r="W56" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="X56" s="2"/>
+      <c r="W56" s="2"/>
+      <c r="X56" s="2" t="s">
+        <v>36</v>
+      </c>
       <c r="Y56" s="2"/>
       <c r="Z56" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="AA56" s="2"/>
+        <v>44</v>
+      </c>
+      <c r="AA56" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="AB56" s="2"/>
       <c r="AC56" s="2"/>
-    </row>
-    <row r="57" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD56" s="2"/>
+    </row>
+    <row r="57" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>341</v>
       </c>
@@ -4414,13 +4453,13 @@
       <c r="E57" s="2"/>
       <c r="F57" s="2"/>
       <c r="G57" s="2" t="s">
-        <v>142</v>
+        <v>28</v>
       </c>
       <c r="H57" s="2" t="s">
-        <v>128</v>
+        <v>32</v>
       </c>
       <c r="I57" s="2" t="s">
-        <v>57</v>
+        <v>33</v>
       </c>
       <c r="J57" s="2"/>
       <c r="K57" s="2"/>
@@ -4430,163 +4469,112 @@
       <c r="O57" s="2"/>
       <c r="P57" s="2"/>
       <c r="Q57" s="2"/>
-      <c r="R57" s="2" t="s">
+      <c r="R57" s="2"/>
+      <c r="S57" s="2" t="s">
         <v>345</v>
       </c>
-      <c r="S57" s="2"/>
-      <c r="T57" s="2"/>
+      <c r="T57" s="2" t="s">
+        <v>346</v>
+      </c>
       <c r="U57" s="2"/>
-      <c r="V57" s="2"/>
-      <c r="W57" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="X57" s="2"/>
-      <c r="Y57" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="Z57" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="AA57" s="2"/>
+      <c r="V57" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="W57" s="2"/>
+      <c r="X57" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y57" s="2"/>
+      <c r="Z57" s="2"/>
+      <c r="AA57" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="AB57" s="2"/>
       <c r="AC57" s="2"/>
-    </row>
-    <row r="58" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A58" s="2" t="s">
-        <v>346</v>
-      </c>
-      <c r="B58" s="2" t="s">
-        <v>347</v>
-      </c>
-      <c r="C58" s="2" t="s">
+      <c r="AD57" s="2"/>
+    </row>
+    <row r="58" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
         <v>348</v>
       </c>
-      <c r="D58" s="2" t="s">
+      <c r="B58" t="s">
+        <v>328</v>
+      </c>
+      <c r="C58" t="s">
         <v>349</v>
       </c>
-      <c r="E58" s="2"/>
-      <c r="F58" s="2"/>
-      <c r="G58" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H58" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="I58" s="2" t="s">
+      <c r="D58" t="s">
+        <v>350</v>
+      </c>
+      <c r="G58" t="s">
+        <v>168</v>
+      </c>
+      <c r="H58" t="s">
+        <v>56</v>
+      </c>
+      <c r="I58" t="s">
+        <v>57</v>
+      </c>
+      <c r="X58" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA58" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="59" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A59" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="E59" s="2"/>
+      <c r="F59" s="2"/>
+      <c r="G59" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="H59" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="I59" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="J58" s="2"/>
-      <c r="K58" s="2"/>
-      <c r="L58" s="2"/>
-      <c r="M58" s="2"/>
-      <c r="N58" s="2"/>
-      <c r="O58" s="2"/>
-      <c r="P58" s="2"/>
-      <c r="Q58" s="2"/>
-      <c r="R58" s="2" t="s">
-        <v>350</v>
-      </c>
-      <c r="S58" s="2" t="s">
-        <v>351</v>
-      </c>
-      <c r="T58" s="2"/>
-      <c r="U58" s="2" t="s">
-        <v>352</v>
-      </c>
-      <c r="V58" s="2"/>
-      <c r="W58" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="X58" s="2"/>
-      <c r="Y58" s="2"/>
-      <c r="Z58" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="AA58" s="2"/>
-      <c r="AB58" s="2"/>
-      <c r="AC58" s="2"/>
-    </row>
-    <row r="59" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>353</v>
-      </c>
-      <c r="B59" t="s">
-        <v>333</v>
-      </c>
-      <c r="C59" t="s">
-        <v>354</v>
-      </c>
-      <c r="D59" t="s">
+      <c r="J59" s="2"/>
+      <c r="K59" s="2"/>
+      <c r="L59" s="2"/>
+      <c r="M59" s="2"/>
+      <c r="N59" s="2"/>
+      <c r="O59" s="2"/>
+      <c r="P59" s="2"/>
+      <c r="Q59" s="2"/>
+      <c r="R59" s="2"/>
+      <c r="S59" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="T59" s="2" t="s">
         <v>355</v>
       </c>
-      <c r="G59" t="s">
-        <v>168</v>
-      </c>
-      <c r="H59" t="s">
-        <v>56</v>
-      </c>
-      <c r="I59" t="s">
-        <v>57</v>
-      </c>
-      <c r="W59" t="s">
-        <v>36</v>
-      </c>
-      <c r="Z59" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="60" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A60" s="2" t="s">
-        <v>356</v>
-      </c>
-      <c r="B60" s="2" t="s">
-        <v>357</v>
-      </c>
-      <c r="C60" s="2" t="s">
-        <v>358</v>
-      </c>
-      <c r="D60" s="2" t="s">
-        <v>359</v>
-      </c>
-      <c r="E60" s="2"/>
-      <c r="F60" s="2"/>
-      <c r="G60" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="H60" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="I60" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="J60" s="2"/>
-      <c r="K60" s="2"/>
-      <c r="L60" s="2"/>
-      <c r="M60" s="2"/>
-      <c r="N60" s="2"/>
-      <c r="O60" s="2"/>
-      <c r="P60" s="2"/>
-      <c r="Q60" s="2"/>
-      <c r="R60" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="S60" s="2" t="s">
-        <v>360</v>
-      </c>
-      <c r="T60" s="2"/>
-      <c r="U60" s="2"/>
-      <c r="V60" s="2"/>
-      <c r="W60" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="X60" s="2"/>
-      <c r="Y60" s="2"/>
-      <c r="Z60" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="AA60" s="2"/>
-      <c r="AB60" s="2"/>
-      <c r="AC60" s="2"/>
+      <c r="U59" s="2"/>
+      <c r="V59" s="2"/>
+      <c r="W59" s="2"/>
+      <c r="X59" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y59" s="2"/>
+      <c r="Z59" s="2"/>
+      <c r="AA59" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="AB59" s="2"/>
+      <c r="AC59" s="2"/>
+      <c r="AD59" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>